<commit_message>
Retro Updated for Last Sprint
</commit_message>
<xml_diff>
--- a/Team-Techies Sprint Task Sheet.xlsx
+++ b/Team-Techies Sprint Task Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="191">
   <si>
     <t>Week #1 (28 hrs / week)</t>
   </si>
@@ -307,7 +307,7 @@
     <t>What didnt go well</t>
   </si>
   <si>
-    <t>Remaining questions</t>
+    <t>Remaining questions/ Should work on</t>
   </si>
   <si>
     <t>Technology Requirements</t>
@@ -467,6 +467,132 @@
   </si>
   <si>
     <t>Building more reliable interactions</t>
+  </si>
+  <si>
+    <t>Retrospective Report for Sprint - 5</t>
+  </si>
+  <si>
+    <t>Started working on major Booking page, User Profile, Change Reservations, add and view, search flights</t>
+  </si>
+  <si>
+    <t>Lot of complexities involved in writing the logics of core functionalites like booking and search flights</t>
+  </si>
+  <si>
+    <t>Learned more about the requirements and have to study about algorithms involved to implement components</t>
+  </si>
+  <si>
+    <t>Also completed working on APIs to get all flights, search and show flights, booking and get booking. Added logger too</t>
+  </si>
+  <si>
+    <t>Working back anf forth with DB and Frontend has been complex and didn't go well at times</t>
+  </si>
+  <si>
+    <t>How to seamlessly integrate and pass the data required to and forth between backend Databases and Frontend</t>
+  </si>
+  <si>
+    <t>Retrospective Report for Sprint - 6</t>
+  </si>
+  <si>
+    <t>Completed the previous challenges and completed working on Frontend for My Bookings, My Profile for customer and frontend for cancelling Admin and Customer</t>
+  </si>
+  <si>
+    <t>Couldn't implement certain functionalities due to time constraints. Postponed some works towards the next sprint</t>
+  </si>
+  <si>
+    <t>Have to manage time well and splitup the prorities balancing the functionality and UI</t>
+  </si>
+  <si>
+    <t>Finished working on Cancel, Change Booking, Purchase seats and get available seats APIs</t>
+  </si>
+  <si>
+    <t>Can't get the idea to use better techniques to build a few functions inside individual API</t>
+  </si>
+  <si>
+    <t>Should learn more multiple and complex endpoints</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Created DBs for Booking and resolved the issues of merge conflicts in DBs along with updating collections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defining and following schemas with error formating has been challenging </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needs to learn more about implementing quickly </t>
+  </si>
+  <si>
+    <t>Retrospective Report for Sprint - 7</t>
+  </si>
+  <si>
+    <t>Minor Code Changes</t>
+  </si>
+  <si>
+    <t>Most of the core functionalities implementation has been successfully implemented. Did minor code changes to decrease dependencies and support data flow</t>
+  </si>
+  <si>
+    <t>One of the ddificult challenges has been to keep the session and data flow. Though the code changes are minor, selective functions and lines were hard to find and change</t>
+  </si>
+  <si>
+    <t>Plan things accordingly and test selected components at before hand. Work more on collaboration and fixing the requirement parameters</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Successfully completed integrating almost all the components locally</t>
+  </si>
+  <si>
+    <t>Certain compoenents are inconsistent to integrate</t>
+  </si>
+  <si>
+    <t>Plan things accordingly and test selected compoenents at before hand. Work more on collaboration and fixing the requirement parameters</t>
+  </si>
+  <si>
+    <t>Retrospective Report for Sprint - 8</t>
+  </si>
+  <si>
+    <t>Resolving Minor Integration Errors</t>
+  </si>
+  <si>
+    <t>Completely done with integration and resolved all the issues</t>
+  </si>
+  <si>
+    <t>Almost all the things did go well as we've been prepared</t>
+  </si>
+  <si>
+    <t>Things went well as expected</t>
+  </si>
+  <si>
+    <t>Successfully deployed on EC2 Autoscale cluster and had it running flawlessly</t>
+  </si>
+  <si>
+    <t>Faced a few security, identity access and dependencies installment issue. Minor to resolve them at hand</t>
+  </si>
+  <si>
+    <t>More about configuring secuirty policies</t>
+  </si>
+  <si>
+    <t>Testing mutliple times with different outputs and system conditions</t>
+  </si>
+  <si>
+    <t>We took care of this aspect so nothing much</t>
+  </si>
+  <si>
+    <t>Nothing as such</t>
+  </si>
+  <si>
+    <t>Retrospection</t>
+  </si>
+  <si>
+    <t>Revised everything from the start, how we carried on, initial agends and final achievements, challenges and pain points, what to work on and how to improve and more.</t>
+  </si>
+  <si>
+    <t>There will always be room for improvements. Learning from those challenges and moving forwardg is the crucial thing.</t>
+  </si>
+  <si>
+    <t>Confidently we can say we achieved what we expected at the rate of 95%.</t>
   </si>
 </sst>
 </file>
@@ -714,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -916,6 +1042,9 @@
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -926,6 +1055,9 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -969,7 +1101,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="7">
+  <tableStyles count="15">
     <tableStyle count="2" pivot="0" name="Retrospective-Sprint-Sheet-style">
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="2" type="secondRowStripe"/>
@@ -983,8 +1115,7 @@
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="Retrospective-Sprint-Sheet-style 4">
-      <tableStyleElement dxfId="3" type="headerRow"/>
+    <tableStyle count="2" pivot="0" name="Retrospective-Sprint-Sheet-style 4">
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
@@ -998,7 +1129,44 @@
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="2" pivot="0" name="Retrospective-Sprint-Sheet-style 7">
+    <tableStyle count="3" pivot="0" name="Retrospective-Sprint-Sheet-style 7">
+      <tableStyleElement dxfId="3" type="headerRow"/>
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Retrospective-Sprint-Sheet-style 8">
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Retrospective-Sprint-Sheet-style 9">
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Retrospective-Sprint-Sheet-style 10">
+      <tableStyleElement dxfId="3" type="headerRow"/>
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Retrospective-Sprint-Sheet-style 11">
+      <tableStyleElement dxfId="3" type="headerRow"/>
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Retrospective-Sprint-Sheet-style 12">
+      <tableStyleElement dxfId="3" type="headerRow"/>
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Retrospective-Sprint-Sheet-style 13">
+      <tableStyleElement dxfId="3" type="headerRow"/>
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Retrospective-Sprint-Sheet-style 14">
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Retrospective-Sprint-Sheet-style 15">
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
@@ -1229,11 +1397,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1016481926"/>
-        <c:axId val="1444428562"/>
+        <c:axId val="764497669"/>
+        <c:axId val="1934674474"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1016481926"/>
+        <c:axId val="764497669"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,10 +1453,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1444428562"/>
+        <c:crossAx val="1934674474"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1444428562"/>
+        <c:axId val="1934674474"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,7 +1531,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1016481926"/>
+        <c:crossAx val="764497669"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1612,11 +1780,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="847496200"/>
-        <c:axId val="1839749112"/>
+        <c:axId val="1088747905"/>
+        <c:axId val="1429129000"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="847496200"/>
+        <c:axId val="1088747905"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1668,10 +1836,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839749112"/>
+        <c:crossAx val="1429129000"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1839749112"/>
+        <c:axId val="1429129000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,7 +1914,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="847496200"/>
+        <c:crossAx val="1088747905"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1996,11 +2164,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1028351600"/>
-        <c:axId val="426745639"/>
+        <c:axId val="1624318999"/>
+        <c:axId val="198965908"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1028351600"/>
+        <c:axId val="1624318999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2052,10 +2220,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426745639"/>
+        <c:crossAx val="198965908"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426745639"/>
+        <c:axId val="198965908"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2130,7 +2298,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028351600"/>
+        <c:crossAx val="1624318999"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2380,11 +2548,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1145828025"/>
-        <c:axId val="671032598"/>
+        <c:axId val="1544471696"/>
+        <c:axId val="522413363"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1145828025"/>
+        <c:axId val="1544471696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2436,10 +2604,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="671032598"/>
+        <c:crossAx val="522413363"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="671032598"/>
+        <c:axId val="522413363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,7 +2682,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1145828025"/>
+        <c:crossAx val="1544471696"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2685,7 +2853,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B15:E18" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B23:E25" displayName="Table_1" id="1">
   <tableColumns count="4">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2696,8 +2864,101 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A14:E14" displayName="Table_10" id="10">
+  <tableColumns count="5">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 10" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A29:E29" displayName="Table_11" id="11">
+  <tableColumns count="5">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 11" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:E2" displayName="Table_12" id="12">
+  <tableColumns count="5">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 12" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A8:E8" displayName="Table_13" id="13">
+  <tableColumns count="5">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 13" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B30:E32" displayName="Table_14" id="14">
+  <tableColumns count="4">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 14" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B9:B11" displayName="Table_15" id="15">
+  <tableColumns count="1">
+    <tableColumn name="Column1" id="1"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 15" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A14:E14" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A22:E22" displayName="Table_2" id="2">
   <tableColumns count="5">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2715,7 +2976,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B23:E25" displayName="Table_3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B49:E52" displayName="Table_3" id="3">
   <tableColumns count="4">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2727,25 +2988,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:E2" displayName="Table_4" id="4">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B43:E45" displayName="Table_4" id="4">
+  <tableColumns count="4">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
     <tableColumn name="Column3" id="3"/>
     <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
   </tableColumns>
   <tableStyleInfo name="Retrospective-Sprint-Sheet-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A22:E22" displayName="Table_5" id="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A48:E48" displayName="Table_5" id="5">
   <tableColumns count="5">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2763,7 +3018,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A8:E8" displayName="Table_6" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A42:E42" displayName="Table_6" id="6">
   <tableColumns count="5">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2781,11 +3036,44 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B9:B11" displayName="Table_7" id="7">
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A35:E35" displayName="Table_7" id="7">
+  <tableColumns count="5">
     <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
   </tableColumns>
   <tableStyleInfo name="Retrospective-Sprint-Sheet-style 7" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B36:E38" displayName="Table_8" id="8">
+  <tableColumns count="4">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 8" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B15:E18" displayName="Table_9" id="9">
+  <tableColumns count="4">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+  </tableColumns>
+  <tableStyleInfo name="Retrospective-Sprint-Sheet-style 9" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -30617,7 +30905,7 @@
       <c r="D8" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="73" t="s">
         <v>95</v>
       </c>
     </row>
@@ -30625,7 +30913,7 @@
       <c r="A9" s="68">
         <v>1.0</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="74" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="69" t="s">
@@ -30642,7 +30930,7 @@
       <c r="A10" s="71">
         <v>2.0</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="72" t="s">
@@ -30659,7 +30947,7 @@
       <c r="A11" s="68">
         <v>3.0</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="75" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="69" t="s">
@@ -30696,7 +30984,7 @@
       <c r="D14" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="73" t="s">
         <v>95</v>
       </c>
     </row>
@@ -30704,16 +30992,16 @@
       <c r="A15" s="68">
         <v>1.0</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="75" t="s">
         <v>123</v>
       </c>
     </row>
@@ -30721,16 +31009,16 @@
       <c r="A16" s="71">
         <v>2.0</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="75" t="s">
+      <c r="E16" s="76" t="s">
         <v>127</v>
       </c>
     </row>
@@ -30738,16 +31026,16 @@
       <c r="A17" s="68">
         <v>3.0</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="74" t="s">
+      <c r="D17" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="74" t="s">
+      <c r="E17" s="75" t="s">
         <v>131</v>
       </c>
     </row>
@@ -30758,37 +31046,37 @@
       <c r="B18" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="75" t="s">
+      <c r="D18" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E18" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="76"/>
-      <c r="R18" s="76"/>
-      <c r="S18" s="76"/>
-      <c r="T18" s="76"/>
-      <c r="U18" s="76"/>
-      <c r="V18" s="76"/>
-      <c r="W18" s="76"/>
-      <c r="X18" s="76"/>
-      <c r="Y18" s="76"/>
-      <c r="Z18" s="76"/>
-      <c r="AA18" s="76"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
+      <c r="K18" s="77"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77"/>
+      <c r="O18" s="77"/>
+      <c r="P18" s="77"/>
+      <c r="Q18" s="77"/>
+      <c r="R18" s="77"/>
+      <c r="S18" s="77"/>
+      <c r="T18" s="77"/>
+      <c r="U18" s="77"/>
+      <c r="V18" s="77"/>
+      <c r="W18" s="77"/>
+      <c r="X18" s="77"/>
+      <c r="Y18" s="77"/>
+      <c r="Z18" s="77"/>
+      <c r="AA18" s="77"/>
     </row>
     <row r="19">
       <c r="A19" s="40"/>
@@ -30796,7 +31084,7 @@
     <row r="20">
       <c r="A20" s="40"/>
     </row>
-    <row r="21">
+    <row r="21" ht="31.5" customHeight="1">
       <c r="A21" s="66" t="s">
         <v>136</v>
       </c>
@@ -30817,7 +31105,7 @@
       <c r="D22" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="67" t="s">
+      <c r="E22" s="73" t="s">
         <v>95</v>
       </c>
     </row>
@@ -30825,16 +31113,16 @@
       <c r="A23" s="68">
         <v>1.0</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="74" t="s">
+      <c r="D23" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="E23" s="74" t="s">
+      <c r="E23" s="75" t="s">
         <v>140</v>
       </c>
     </row>
@@ -30842,16 +31130,16 @@
       <c r="A24" s="71">
         <v>2.0</v>
       </c>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="75" t="s">
+      <c r="E24" s="76" t="s">
         <v>144</v>
       </c>
     </row>
@@ -30859,16 +31147,16 @@
       <c r="A25" s="68">
         <v>3.0</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="74" t="s">
+      <c r="D25" s="75" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="75" t="s">
         <v>148</v>
       </c>
     </row>
@@ -30878,38 +31166,150 @@
     <row r="27">
       <c r="A27" s="40"/>
     </row>
-    <row r="28">
-      <c r="A28" s="40"/>
+    <row r="28" ht="24.0" customHeight="1">
+      <c r="A28" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29">
-      <c r="A29" s="40"/>
+      <c r="A29" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="40"/>
+      <c r="A30" s="68">
+        <v>1.0</v>
+      </c>
+      <c r="B30" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="40"/>
+      <c r="A31" s="71">
+        <v>2.0</v>
+      </c>
+      <c r="B31" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="76" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="40"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
     </row>
     <row r="33">
       <c r="A33" s="40"/>
     </row>
     <row r="34">
-      <c r="A34" s="40"/>
+      <c r="A34" s="66" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
     </row>
     <row r="35">
-      <c r="A35" s="40"/>
+      <c r="A35" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="73" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="40"/>
+      <c r="A36" s="68">
+        <v>1.0</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="75" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="75" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="40"/>
+      <c r="A37" s="71">
+        <v>2.0</v>
+      </c>
+      <c r="B37" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="76" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" s="76" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="40"/>
+      <c r="A38" s="68">
+        <v>3.0</v>
+      </c>
+      <c r="B38" s="75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="76" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="40"/>
@@ -30917,41 +31317,167 @@
     <row r="40">
       <c r="A40" s="40"/>
     </row>
-    <row r="41">
-      <c r="A41" s="40"/>
+    <row r="41" ht="24.75" customHeight="1">
+      <c r="A41" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
     </row>
     <row r="42">
-      <c r="A42" s="40"/>
+      <c r="A42" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="73" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="40"/>
+      <c r="A43" s="68">
+        <v>1.0</v>
+      </c>
+      <c r="B43" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" s="75" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="40"/>
+      <c r="A44" s="71">
+        <v>2.0</v>
+      </c>
+      <c r="B44" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="76" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="76" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="40"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="75"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
     </row>
     <row r="46">
       <c r="A46" s="40"/>
     </row>
     <row r="47">
-      <c r="A47" s="40"/>
+      <c r="A47" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
     </row>
     <row r="48">
-      <c r="A48" s="40"/>
+      <c r="A48" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="73" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="40"/>
+      <c r="A49" s="68">
+        <v>1.0</v>
+      </c>
+      <c r="B49" s="75" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="75" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" s="75" t="s">
+        <v>179</v>
+      </c>
+      <c r="E49" s="75" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="40"/>
+      <c r="A50" s="71">
+        <v>2.0</v>
+      </c>
+      <c r="B50" s="75" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="76" t="s">
+        <v>181</v>
+      </c>
+      <c r="D50" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="E50" s="76" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="40"/>
+      <c r="A51" s="68">
+        <v>3.0</v>
+      </c>
+      <c r="B51" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="75" t="s">
+        <v>184</v>
+      </c>
+      <c r="D51" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="40"/>
+      <c r="A52" s="71">
+        <v>4.0</v>
+      </c>
+      <c r="B52" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="C52" s="76" t="s">
+        <v>188</v>
+      </c>
+      <c r="D52" s="78" t="s">
+        <v>189</v>
+      </c>
+      <c r="E52" s="75" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="40"/>
@@ -33720,21 +34246,33 @@
       <c r="A974" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A47:B47"/>
   </mergeCells>
   <drawing r:id="rId1"/>
-  <tableParts count="7">
-    <tablePart r:id="rId9"/>
-    <tablePart r:id="rId10"/>
-    <tablePart r:id="rId11"/>
-    <tablePart r:id="rId12"/>
-    <tablePart r:id="rId13"/>
-    <tablePart r:id="rId14"/>
-    <tablePart r:id="rId15"/>
+  <tableParts count="15">
+    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId28"/>
+    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Final Task sheet + Burnd down + Retrospective Sprint
</commit_message>
<xml_diff>
--- a/Team-Techies Sprint Task Sheet.xlsx
+++ b/Team-Techies Sprint Task Sheet.xlsx
@@ -187,7 +187,7 @@
     <t>Wireframe for Landing, Search flights, Bookings</t>
   </si>
   <si>
-    <t>Models and API for AirCraft,  Add and Get Airport,</t>
+    <t>Models and API for AirCraft,  Add and Get Airport</t>
   </si>
   <si>
     <t>Models and API Add Flight, Search Flights</t>
@@ -840,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1014,7 +1014,6 @@
     <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -1397,11 +1396,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="764497669"/>
-        <c:axId val="1934674474"/>
+        <c:axId val="683545777"/>
+        <c:axId val="1042012497"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="764497669"/>
+        <c:axId val="683545777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,10 +1452,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934674474"/>
+        <c:crossAx val="1042012497"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1934674474"/>
+        <c:axId val="1042012497"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1530,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="764497669"/>
+        <c:crossAx val="683545777"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1780,11 +1779,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1088747905"/>
-        <c:axId val="1429129000"/>
+        <c:axId val="549246164"/>
+        <c:axId val="1870073617"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1088747905"/>
+        <c:axId val="549246164"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,10 +1835,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429129000"/>
+        <c:crossAx val="1870073617"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1429129000"/>
+        <c:axId val="1870073617"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1914,7 +1913,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1088747905"/>
+        <c:crossAx val="549246164"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2164,11 +2163,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1624318999"/>
-        <c:axId val="198965908"/>
+        <c:axId val="1687324624"/>
+        <c:axId val="1535334712"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1624318999"/>
+        <c:axId val="1687324624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2220,10 +2219,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198965908"/>
+        <c:crossAx val="1535334712"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198965908"/>
+        <c:axId val="1535334712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2298,7 +2297,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1624318999"/>
+        <c:crossAx val="1687324624"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2364,7 +2363,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint-1'!$E$6</c:f>
+              <c:f>'Sprint-3'!$E$6</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2381,7 +2380,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint-1'!$F$6:$K$6</c:f>
+              <c:f>'Sprint-3'!$F$6:$K$6</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2391,7 +2390,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint-1'!$E$7</c:f>
+              <c:f>'Sprint-3'!$E$7</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2408,7 +2407,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint-1'!$F$7:$K$7</c:f>
+              <c:f>'Sprint-3'!$F$7:$K$7</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2418,7 +2417,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint-1'!$E$8</c:f>
+              <c:f>'Sprint-3'!$E$8</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2435,7 +2434,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint-1'!$F$8:$K$8</c:f>
+              <c:f>'Sprint-3'!$F$8:$K$8</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2445,7 +2444,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint-1'!$E$9</c:f>
+              <c:f>'Sprint-3'!$E$9</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2462,7 +2461,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint-1'!$F$9:$K$9</c:f>
+              <c:f>'Sprint-3'!$F$9:$K$9</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2472,7 +2471,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint-1'!$E$10</c:f>
+              <c:f>'Sprint-3'!$E$10</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2489,7 +2488,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint-1'!$F$10:$K$10</c:f>
+              <c:f>'Sprint-3'!$F$10:$K$10</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2499,7 +2498,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint-1'!$E$11</c:f>
+              <c:f>'Sprint-3'!$E$11</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2516,7 +2515,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint-1'!$F$11:$K$11</c:f>
+              <c:f>'Sprint-3'!$F$11:$K$11</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2526,7 +2525,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint-1'!$E$12</c:f>
+              <c:f>'Sprint-3'!$E$12</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2543,16 +2542,16 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint-1'!$F$12:$K$12</c:f>
+              <c:f>'Sprint-3'!$F$12:$K$12</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1544471696"/>
-        <c:axId val="522413363"/>
+        <c:axId val="1790425266"/>
+        <c:axId val="1954478024"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1544471696"/>
+        <c:axId val="1790425266"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2604,10 +2603,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522413363"/>
+        <c:crossAx val="1954478024"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="522413363"/>
+        <c:axId val="1954478024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2682,7 +2681,1916 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1544471696"/>
+        <c:crossAx val="1790425266"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart - Sprint 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$6</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4285F4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$6:$K$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$7</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DB4437">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DB4437"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$7:$K$7</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$8</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F4B400">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="F4B400"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$8:$K$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$9</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0F9D58">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="0F9D58"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$9:$K$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$10</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF6D00">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$10:$K$10</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$11</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="46BDC6">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="46BDC6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$11:$K$11</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="AB30C4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="AB30C4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$12:$K$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-4'!$E$13</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C1BC1F">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="C1BC1F"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-4'!$F$13:$K$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="552951940"/>
+        <c:axId val="831136648"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="552951940"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="831136648"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="831136648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Hours of Work Remaining </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552951940"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart - Sprint 5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$6</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4285F4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$6:$K$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$7</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DB4437">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DB4437"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$7:$K$7</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$8</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F4B400">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="F4B400"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$8:$K$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$9</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0F9D58">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="0F9D58"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$9:$K$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$10</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF6D00">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$10:$K$10</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$11</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="46BDC6">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="46BDC6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$11:$K$11</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="AB30C4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="AB30C4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$12:$K$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-5'!$E$13</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C1BC1F">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="C1BC1F"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-5'!$F$13:$K$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="15374237"/>
+        <c:axId val="1346628175"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="15374237"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1346628175"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1346628175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Hours of Work Remaining </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15374237"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart - Sprint 6</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$6</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4285F4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$6:$K$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$7</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DB4437">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DB4437"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$7:$K$7</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$8</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F4B400">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="F4B400"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$8:$K$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$9</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0F9D58">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="0F9D58"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$9:$K$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$10</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF6D00">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$10:$K$10</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$11</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="46BDC6">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="46BDC6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$11:$K$11</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="AB30C4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="AB30C4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$12:$K$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-6'!$E$13</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C1BC1F">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="C1BC1F"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-6'!$F$13:$K$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="801578985"/>
+        <c:axId val="1570900865"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="801578985"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1570900865"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1570900865"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Hours of Work Remaining </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="801578985"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart - Sprint 7</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.030888290713324364"/>
+          <c:y val="0.04782135076252724"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-7'!$E$6</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4285F4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-7'!$F$6:$K$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-7'!$E$7</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DB4437">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DB4437"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-7'!$F$7:$K$7</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-7'!$E$8</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F4B400">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="F4B400"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-7'!$F$8:$K$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-7'!$E$9</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0F9D58">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="0F9D58"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-7'!$F$9:$K$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-7'!$E$10</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF6D00">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-7'!$F$10:$K$10</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1517895834"/>
+        <c:axId val="1446274857"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="1517895834"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1446274857"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1446274857"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Hours of Work Remaining </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1517895834"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart - Sprint 8</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.030888290713324364"/>
+          <c:y val="0.04564270152505447"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-8'!$E$6</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4285F4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-8'!$F$6:$K$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-8'!$E$7</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DB4437">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DB4437"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-8'!$F$7:$K$7</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-8'!$E$8</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F4B400">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="F4B400"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-8'!$F$8:$K$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-8'!$E$9</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0F9D58">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="0F9D58"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-8'!$F$9:$K$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-8'!$E$10</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF6D00">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-8'!$F$10:$K$10</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="691014957"/>
+        <c:axId val="654942359"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="691014957"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654942359"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="654942359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Hours of Work Remaining </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="691014957"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2806,12 +4714,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3514725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:ext cx="7077075" cy="4371975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
@@ -2833,23 +4741,153 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7077075" cy="4371975"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7077075" cy="4371975"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7077075" cy="4371975"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7077075" cy="4371975"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 8" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7077075" cy="4371975"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 9" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30718,7 +32756,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="65" t="s">
         <v>90</v>
       </c>
       <c r="C1" s="28"/>
@@ -30726,19 +32764,19 @@
       <c r="E1" s="28"/>
     </row>
     <row r="2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="66" t="s">
         <v>95</v>
       </c>
       <c r="F2" s="40"/>
@@ -30765,127 +32803,127 @@
       <c r="AA2" s="40"/>
     </row>
     <row r="3" ht="60.75" customHeight="1">
-      <c r="A3" s="68">
+      <c r="A3" s="67">
         <v>1.0</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="69" t="s">
+      <c r="E3" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="69"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="69"/>
     </row>
     <row r="4" ht="39.0" customHeight="1">
-      <c r="A4" s="71">
+      <c r="A4" s="70">
         <v>2.0</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="69"/>
+      <c r="W4" s="69"/>
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="69"/>
+      <c r="AA4" s="69"/>
     </row>
     <row r="5">
-      <c r="A5" s="68">
+      <c r="A5" s="67">
         <v>3.0</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="68" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
+      <c r="Y5" s="69"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
     </row>
     <row r="6" ht="26.25" customHeight="1">
       <c r="A6" s="40"/>
     </row>
     <row r="7" ht="36.75" customHeight="1">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="65" t="s">
         <v>108</v>
       </c>
       <c r="C7" s="28"/>
@@ -30893,70 +32931,70 @@
       <c r="E7" s="28"/>
     </row>
     <row r="8">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="72" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="68">
+      <c r="A9" s="67">
         <v>1.0</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="68" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="71">
+      <c r="A10" s="70">
         <v>2.0</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="71" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="11" ht="32.25" customHeight="1">
-      <c r="A11" s="68">
+      <c r="A11" s="67">
         <v>3.0</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="68" t="s">
         <v>118</v>
       </c>
     </row>
@@ -30964,7 +33002,7 @@
       <c r="A12" s="40"/>
     </row>
     <row r="13" ht="36.75" customHeight="1">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="65" t="s">
         <v>119</v>
       </c>
       <c r="C13" s="28"/>
@@ -30972,111 +33010,111 @@
       <c r="E13" s="28"/>
     </row>
     <row r="14">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="E14" s="72" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="68">
+      <c r="A15" s="67">
         <v>1.0</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="74" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="71">
+      <c r="A16" s="70">
         <v>2.0</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="76" t="s">
+      <c r="C16" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="76" t="s">
+      <c r="D16" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="76" t="s">
+      <c r="E16" s="75" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="17" ht="41.25" customHeight="1">
-      <c r="A17" s="68">
+      <c r="A17" s="67">
         <v>3.0</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="75" t="s">
+      <c r="D17" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="75" t="s">
+      <c r="E17" s="74" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="71">
+      <c r="A18" s="70">
         <v>4.0</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="76" t="s">
+      <c r="C18" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="76" t="s">
+      <c r="D18" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="76" t="s">
+      <c r="E18" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="77"/>
-      <c r="N18" s="77"/>
-      <c r="O18" s="77"/>
-      <c r="P18" s="77"/>
-      <c r="Q18" s="77"/>
-      <c r="R18" s="77"/>
-      <c r="S18" s="77"/>
-      <c r="T18" s="77"/>
-      <c r="U18" s="77"/>
-      <c r="V18" s="77"/>
-      <c r="W18" s="77"/>
-      <c r="X18" s="77"/>
-      <c r="Y18" s="77"/>
-      <c r="Z18" s="77"/>
-      <c r="AA18" s="77"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="76"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="76"/>
+      <c r="P18" s="76"/>
+      <c r="Q18" s="76"/>
+      <c r="R18" s="76"/>
+      <c r="S18" s="76"/>
+      <c r="T18" s="76"/>
+      <c r="U18" s="76"/>
+      <c r="V18" s="76"/>
+      <c r="W18" s="76"/>
+      <c r="X18" s="76"/>
+      <c r="Y18" s="76"/>
+      <c r="Z18" s="76"/>
+      <c r="AA18" s="76"/>
     </row>
     <row r="19">
       <c r="A19" s="40"/>
@@ -31085,7 +33123,7 @@
       <c r="A20" s="40"/>
     </row>
     <row r="21" ht="31.5" customHeight="1">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="65" t="s">
         <v>136</v>
       </c>
       <c r="C21" s="28"/>
@@ -31093,70 +33131,70 @@
       <c r="E21" s="28"/>
     </row>
     <row r="22">
-      <c r="A22" s="67" t="s">
+      <c r="A22" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="73" t="s">
+      <c r="E22" s="72" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="68">
+      <c r="A23" s="67">
         <v>1.0</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="75" t="s">
+      <c r="D23" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="E23" s="75" t="s">
+      <c r="E23" s="74" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="71">
+      <c r="A24" s="70">
         <v>2.0</v>
       </c>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="76" t="s">
+      <c r="C24" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="76" t="s">
+      <c r="D24" s="75" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="76" t="s">
+      <c r="E24" s="75" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="68">
+      <c r="A25" s="67">
         <v>3.0</v>
       </c>
-      <c r="B25" s="75" t="s">
+      <c r="B25" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="75" t="s">
+      <c r="D25" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="75" t="s">
+      <c r="E25" s="74" t="s">
         <v>148</v>
       </c>
     </row>
@@ -31167,7 +33205,7 @@
       <c r="A27" s="40"/>
     </row>
     <row r="28" ht="24.0" customHeight="1">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="65" t="s">
         <v>149</v>
       </c>
       <c r="C28" s="28"/>
@@ -31175,68 +33213,68 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29">
-      <c r="A29" s="67" t="s">
+      <c r="A29" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="67" t="s">
+      <c r="D29" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E29" s="73" t="s">
+      <c r="E29" s="72" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="68">
+      <c r="A30" s="67">
         <v>1.0</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="E30" s="75" t="s">
+      <c r="E30" s="74" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="71">
+      <c r="A31" s="70">
         <v>2.0</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="76" t="s">
+      <c r="D31" s="75" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="76" t="s">
+      <c r="E31" s="75" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="68"/>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
     </row>
     <row r="33">
       <c r="A33" s="40"/>
     </row>
     <row r="34">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="65" t="s">
         <v>156</v>
       </c>
       <c r="C34" s="28"/>
@@ -31244,70 +33282,70 @@
       <c r="E34" s="28"/>
     </row>
     <row r="35">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="67" t="s">
+      <c r="B35" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="67" t="s">
+      <c r="C35" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="67" t="s">
+      <c r="D35" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="73" t="s">
+      <c r="E35" s="72" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="68">
+      <c r="A36" s="67">
         <v>1.0</v>
       </c>
-      <c r="B36" s="75" t="s">
+      <c r="B36" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="D36" s="75" t="s">
+      <c r="D36" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="E36" s="75" t="s">
+      <c r="E36" s="74" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="71">
+      <c r="A37" s="70">
         <v>2.0</v>
       </c>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="76" t="s">
+      <c r="C37" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="D37" s="76" t="s">
+      <c r="D37" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="76" t="s">
+      <c r="E37" s="75" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="68">
+      <c r="A38" s="67">
         <v>3.0</v>
       </c>
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="C38" s="76" t="s">
+      <c r="C38" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="D38" s="76" t="s">
+      <c r="D38" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="E38" s="76" t="s">
+      <c r="E38" s="75" t="s">
         <v>166</v>
       </c>
     </row>
@@ -31318,7 +33356,7 @@
       <c r="A40" s="40"/>
     </row>
     <row r="41" ht="24.75" customHeight="1">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="65" t="s">
         <v>167</v>
       </c>
       <c r="C41" s="28"/>
@@ -31326,68 +33364,68 @@
       <c r="E41" s="28"/>
     </row>
     <row r="42">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="C42" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="67" t="s">
+      <c r="D42" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="73" t="s">
+      <c r="E42" s="72" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="68">
+      <c r="A43" s="67">
         <v>1.0</v>
       </c>
-      <c r="B43" s="75" t="s">
+      <c r="B43" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="C43" s="75" t="s">
+      <c r="C43" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="D43" s="75" t="s">
+      <c r="D43" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="E43" s="75" t="s">
+      <c r="E43" s="74" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="71">
+      <c r="A44" s="70">
         <v>2.0</v>
       </c>
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="C44" s="76" t="s">
+      <c r="C44" s="75" t="s">
         <v>173</v>
       </c>
-      <c r="D44" s="76" t="s">
+      <c r="D44" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="E44" s="76" t="s">
+      <c r="E44" s="75" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="68"/>
-      <c r="B45" s="75"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="76"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="74"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
     </row>
     <row r="46">
       <c r="A46" s="40"/>
     </row>
     <row r="47">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="65" t="s">
         <v>176</v>
       </c>
       <c r="C47" s="28"/>
@@ -31395,87 +33433,87 @@
       <c r="E47" s="28"/>
     </row>
     <row r="48">
-      <c r="A48" s="67" t="s">
+      <c r="A48" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="67" t="s">
+      <c r="B48" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="67" t="s">
+      <c r="C48" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="67" t="s">
+      <c r="D48" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="73" t="s">
+      <c r="E48" s="72" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="68">
+      <c r="A49" s="67">
         <v>1.0</v>
       </c>
-      <c r="B49" s="75" t="s">
+      <c r="B49" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="C49" s="75" t="s">
+      <c r="C49" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="D49" s="75" t="s">
+      <c r="D49" s="74" t="s">
         <v>179</v>
       </c>
-      <c r="E49" s="75" t="s">
+      <c r="E49" s="74" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="71">
+      <c r="A50" s="70">
         <v>2.0</v>
       </c>
-      <c r="B50" s="75" t="s">
+      <c r="B50" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="76" t="s">
+      <c r="C50" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="D50" s="76" t="s">
+      <c r="D50" s="75" t="s">
         <v>182</v>
       </c>
-      <c r="E50" s="76" t="s">
+      <c r="E50" s="75" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="68">
+      <c r="A51" s="67">
         <v>3.0</v>
       </c>
-      <c r="B51" s="75" t="s">
+      <c r="B51" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="75" t="s">
+      <c r="C51" s="74" t="s">
         <v>184</v>
       </c>
-      <c r="D51" s="75" t="s">
+      <c r="D51" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="E51" s="75" t="s">
+      <c r="E51" s="74" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="71">
+      <c r="A52" s="70">
         <v>4.0</v>
       </c>
-      <c r="B52" s="75" t="s">
+      <c r="B52" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="C52" s="76" t="s">
+      <c r="C52" s="75" t="s">
         <v>188</v>
       </c>
-      <c r="D52" s="78" t="s">
+      <c r="D52" s="77" t="s">
         <v>189</v>
       </c>
-      <c r="E52" s="75" t="s">
+      <c r="E52" s="74" t="s">
         <v>190</v>
       </c>
     </row>
@@ -48198,27 +50236,27 @@
       <c r="E14" s="62">
         <v>28.0</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="53">
         <f t="shared" ref="F14:K14" si="1">SUM(F6:F13)</f>
         <v>27</v>
       </c>
-      <c r="G14" s="63">
+      <c r="G14" s="53">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H14" s="63">
+      <c r="H14" s="53">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I14" s="63">
+      <c r="I14" s="53">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J14" s="63">
+      <c r="J14" s="53">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K14" s="63">
+      <c r="K14" s="53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -51581,36 +53619,36 @@
     </row>
     <row r="10">
       <c r="A10" s="38"/>
-      <c r="B10" s="64"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="40"/>
       <c r="D10" s="37">
         <v>28.0</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="64">
         <f t="shared" ref="E10:K10" si="1">SUM(E6:E9)</f>
         <v>28</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="64">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="64">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="H10" s="65">
+      <c r="H10" s="64">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I10" s="65">
+      <c r="I10" s="64">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J10" s="65">
+      <c r="J10" s="64">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K10" s="65">
+      <c r="K10" s="64">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -52035,36 +54073,36 @@
     </row>
     <row r="10">
       <c r="A10" s="38"/>
-      <c r="B10" s="64"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="40"/>
       <c r="D10" s="37">
         <v>28.0</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="64">
         <f t="shared" ref="E10:K10" si="1">SUM(E6:E9)</f>
         <v>28</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="64">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="64">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H10" s="65">
+      <c r="H10" s="64">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I10" s="65">
+      <c r="I10" s="64">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J10" s="65">
+      <c r="J10" s="64">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K10" s="65">
+      <c r="K10" s="64">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>

</xml_diff>